<commit_message>
Combat Shields (Continued) 수정
#645
</commit_message>
<xml_diff>
--- a/Data/Mlie/Combat Shields (Continued) - 2983650634/2983650634.xlsx
+++ b/Data/Mlie/Combat Shields (Continued) - 2983650634/2983650634.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\Combat Shields (Continued) - 2983650634\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.7.3\Combat Shields (Continued) - 2983650634\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151946F4-EA25-457A-B18C-30B8704A740E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE48D58-2DA7-4227-B0CF-A470CC9518B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Merge_RKTM" sheetId="2" r:id="rId2"/>
+    <sheet name="Main_240407" sheetId="3" r:id="rId1"/>
+    <sheet name="231126" sheetId="1" r:id="rId2"/>
+    <sheet name="Merge_RKTM" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="241">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -731,13 +732,49 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>The mod now has settings to change what ranged weapons can be used with shields.
+Weapons can also be limited to be used with light shields only.
+Hopefully this will simplify compatibility with other mods.
+The mod should now also work better when using mods that changes apparel categories.</t>
+  </si>
+  <si>
+    <t>CombatShields_1_4_3.content</t>
+  </si>
+  <si>
+    <t>TabulaRasa.UpdateDef</t>
+  </si>
+  <si>
+    <t>TabulaRasa.UpdateDef+CombatShields_1_4_3.content</t>
+  </si>
+  <si>
+    <t>Korean (한국어) [Translation]</t>
+  </si>
+  <si>
+    <t>English [Source string]</t>
+  </si>
+  <si>
+    <t>Required Mods [Not chosen]</t>
+  </si>
+  <si>
+    <t>전술 방패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carapace shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐러페이스 실드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,6 +788,18 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -790,18 +839,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="1" xr:uid="{D3F774CE-FA40-4BAE-BF37-79E4651785FD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1100,11 +1152,719 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DF3CD5-0DF0-4D18-A6FB-29B06D65B166}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4140625" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="48.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.9140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="29.58203125" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.4140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1957,7 +2717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51003A-E4EB-43BA-A0AA-FC001BF7AE8A}">
   <dimension ref="A1:E63"/>
   <sheetViews>
@@ -1996,7 +2756,7 @@
         <v>128</v>
       </c>
       <c r="E2" t="e">
-        <f>MATCH(A2,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A2,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2012,7 +2772,7 @@
         <v>130</v>
       </c>
       <c r="E3" t="e">
-        <f>MATCH(A3,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A3,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2028,7 +2788,7 @@
         <v>132</v>
       </c>
       <c r="E4" t="e">
-        <f>MATCH(A4,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A4,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2044,7 +2804,7 @@
         <v>134</v>
       </c>
       <c r="E5" t="e">
-        <f>MATCH(A5,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A5,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2060,7 +2820,7 @@
         <v>136</v>
       </c>
       <c r="E6" t="e">
-        <f>MATCH(A6,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A6,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2076,7 +2836,7 @@
         <v>138</v>
       </c>
       <c r="E7" t="e">
-        <f>MATCH(A7,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A7,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2092,7 +2852,7 @@
         <v>140</v>
       </c>
       <c r="E8" t="e">
-        <f>MATCH(A8,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A8,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2108,7 +2868,7 @@
         <v>142</v>
       </c>
       <c r="E9" t="e">
-        <f>MATCH(A9,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A9,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2124,7 +2884,7 @@
         <v>144</v>
       </c>
       <c r="E10" t="e">
-        <f>MATCH(A10,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A10,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2140,7 +2900,7 @@
         <v>146</v>
       </c>
       <c r="E11" t="e">
-        <f>MATCH(A11,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A11,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2156,7 +2916,7 @@
         <v>148</v>
       </c>
       <c r="E12" t="e">
-        <f>MATCH(A12,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A12,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2172,7 +2932,7 @@
         <v>150</v>
       </c>
       <c r="E13" t="e">
-        <f>MATCH(A13,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A13,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2188,7 +2948,7 @@
         <v>152</v>
       </c>
       <c r="E14" t="e">
-        <f>MATCH(A14,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A14,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2204,7 +2964,7 @@
         <v>154</v>
       </c>
       <c r="E15" t="e">
-        <f>MATCH(A15,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A15,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2220,7 +2980,7 @@
         <v>156</v>
       </c>
       <c r="E16" t="e">
-        <f>MATCH(A16,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A16,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2236,7 +2996,7 @@
         <v>158</v>
       </c>
       <c r="E17" t="e">
-        <f>MATCH(A17,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A17,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2252,7 +3012,7 @@
         <v>160</v>
       </c>
       <c r="E18" t="e">
-        <f>MATCH(A18,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A18,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2268,7 +3028,7 @@
         <v>162</v>
       </c>
       <c r="E19" t="e">
-        <f>MATCH(A19,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A19,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2284,7 +3044,7 @@
         <v>164</v>
       </c>
       <c r="E20" t="e">
-        <f>MATCH(A20,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A20,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2300,7 +3060,7 @@
         <v>166</v>
       </c>
       <c r="E21" t="e">
-        <f>MATCH(A21,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A21,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2316,7 +3076,7 @@
         <v>168</v>
       </c>
       <c r="E22" t="e">
-        <f>MATCH(A22,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A22,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2332,7 +3092,7 @@
         <v>170</v>
       </c>
       <c r="E23" t="e">
-        <f>MATCH(A23,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A23,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2348,7 +3108,7 @@
         <v>172</v>
       </c>
       <c r="E24" t="e">
-        <f>MATCH(A24,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A24,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2364,7 +3124,7 @@
         <v>174</v>
       </c>
       <c r="E25" t="e">
-        <f>MATCH(A25,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A25,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2380,7 +3140,7 @@
         <v>176</v>
       </c>
       <c r="E26" t="e">
-        <f>MATCH(A26,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A26,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2396,7 +3156,7 @@
         <v>178</v>
       </c>
       <c r="E27" t="e">
-        <f>MATCH(A27,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A27,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2412,7 +3172,7 @@
         <v>180</v>
       </c>
       <c r="E28" t="e">
-        <f>MATCH(A28,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A28,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2428,7 +3188,7 @@
         <v>182</v>
       </c>
       <c r="E29" t="e">
-        <f>MATCH(A29,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A29,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2444,7 +3204,7 @@
         <v>184</v>
       </c>
       <c r="E30" t="e">
-        <f>MATCH(A30,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A30,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2460,7 +3220,7 @@
         <v>186</v>
       </c>
       <c r="E31" t="e">
-        <f>MATCH(A31,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A31,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2476,7 +3236,7 @@
         <v>188</v>
       </c>
       <c r="E32" t="e">
-        <f>MATCH(A32,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A32,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2492,7 +3252,7 @@
         <v>190</v>
       </c>
       <c r="E33" t="e">
-        <f>MATCH(A33,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A33,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2508,7 +3268,7 @@
         <v>192</v>
       </c>
       <c r="E34" t="e">
-        <f>MATCH(A34,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A34,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2524,7 +3284,7 @@
         <v>194</v>
       </c>
       <c r="E35" t="e">
-        <f>MATCH(A35,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A35,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2540,7 +3300,7 @@
         <v>196</v>
       </c>
       <c r="E36" t="e">
-        <f>MATCH(A36,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A36,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2556,7 +3316,7 @@
         <v>198</v>
       </c>
       <c r="E37" t="e">
-        <f>MATCH(A37,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A37,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2572,7 +3332,7 @@
         <v>200</v>
       </c>
       <c r="E38" t="e">
-        <f>MATCH(A38,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A38,'231126'!$A$2:$A$39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2588,7 +3348,7 @@
         <v>201</v>
       </c>
       <c r="E39">
-        <f>MATCH(A39,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A39,'231126'!$A$2:$A$39,0)</f>
         <v>2</v>
       </c>
     </row>
@@ -2604,7 +3364,7 @@
         <v>202</v>
       </c>
       <c r="E40">
-        <f>MATCH(A40,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A40,'231126'!$A$2:$A$39,0)</f>
         <v>8</v>
       </c>
     </row>
@@ -2620,7 +3380,7 @@
         <v>203</v>
       </c>
       <c r="E41">
-        <f>MATCH(A41,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A41,'231126'!$A$2:$A$39,0)</f>
         <v>12</v>
       </c>
     </row>
@@ -2636,7 +3396,7 @@
         <v>204</v>
       </c>
       <c r="E42">
-        <f>MATCH(A42,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A42,'231126'!$A$2:$A$39,0)</f>
         <v>10</v>
       </c>
     </row>
@@ -2652,7 +3412,7 @@
         <v>205</v>
       </c>
       <c r="E43">
-        <f>MATCH(A43,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A43,'231126'!$A$2:$A$39,0)</f>
         <v>28</v>
       </c>
     </row>
@@ -2668,7 +3428,7 @@
         <v>206</v>
       </c>
       <c r="E44">
-        <f>MATCH(A44,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A44,'231126'!$A$2:$A$39,0)</f>
         <v>16</v>
       </c>
     </row>
@@ -2684,7 +3444,7 @@
         <v>207</v>
       </c>
       <c r="E45">
-        <f>MATCH(A45,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A45,'231126'!$A$2:$A$39,0)</f>
         <v>14</v>
       </c>
     </row>
@@ -2700,7 +3460,7 @@
         <v>208</v>
       </c>
       <c r="E46">
-        <f>MATCH(A46,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A46,'231126'!$A$2:$A$39,0)</f>
         <v>18</v>
       </c>
     </row>
@@ -2716,7 +3476,7 @@
         <v>209</v>
       </c>
       <c r="E47">
-        <f>MATCH(A47,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A47,'231126'!$A$2:$A$39,0)</f>
         <v>22</v>
       </c>
     </row>
@@ -2732,7 +3492,7 @@
         <v>210</v>
       </c>
       <c r="E48">
-        <f>MATCH(A48,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A48,'231126'!$A$2:$A$39,0)</f>
         <v>4</v>
       </c>
     </row>
@@ -2748,7 +3508,7 @@
         <v>211</v>
       </c>
       <c r="E49">
-        <f>MATCH(A49,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A49,'231126'!$A$2:$A$39,0)</f>
         <v>6</v>
       </c>
     </row>
@@ -2764,7 +3524,7 @@
         <v>212</v>
       </c>
       <c r="E50">
-        <f>MATCH(A50,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A50,'231126'!$A$2:$A$39,0)</f>
         <v>24</v>
       </c>
     </row>
@@ -2780,7 +3540,7 @@
         <v>213</v>
       </c>
       <c r="E51">
-        <f>MATCH(A51,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A51,'231126'!$A$2:$A$39,0)</f>
         <v>20</v>
       </c>
     </row>
@@ -2796,7 +3556,7 @@
         <v>214</v>
       </c>
       <c r="E52">
-        <f>MATCH(A52,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A52,'231126'!$A$2:$A$39,0)</f>
         <v>7</v>
       </c>
     </row>
@@ -2812,7 +3572,7 @@
         <v>215</v>
       </c>
       <c r="E53">
-        <f>MATCH(A53,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A53,'231126'!$A$2:$A$39,0)</f>
         <v>23</v>
       </c>
     </row>
@@ -2828,7 +3588,7 @@
         <v>216</v>
       </c>
       <c r="E54">
-        <f>MATCH(A54,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A54,'231126'!$A$2:$A$39,0)</f>
         <v>27</v>
       </c>
     </row>
@@ -2844,7 +3604,7 @@
         <v>217</v>
       </c>
       <c r="E55">
-        <f>MATCH(A55,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A55,'231126'!$A$2:$A$39,0)</f>
         <v>19</v>
       </c>
     </row>
@@ -2860,7 +3620,7 @@
         <v>218</v>
       </c>
       <c r="E56">
-        <f>MATCH(A56,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A56,'231126'!$A$2:$A$39,0)</f>
         <v>15</v>
       </c>
     </row>
@@ -2876,7 +3636,7 @@
         <v>219</v>
       </c>
       <c r="E57">
-        <f>MATCH(A57,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A57,'231126'!$A$2:$A$39,0)</f>
         <v>13</v>
       </c>
     </row>
@@ -2892,7 +3652,7 @@
         <v>220</v>
       </c>
       <c r="E58">
-        <f>MATCH(A58,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A58,'231126'!$A$2:$A$39,0)</f>
         <v>3</v>
       </c>
     </row>
@@ -2908,7 +3668,7 @@
         <v>221</v>
       </c>
       <c r="E59">
-        <f>MATCH(A59,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A59,'231126'!$A$2:$A$39,0)</f>
         <v>11</v>
       </c>
     </row>
@@ -2924,7 +3684,7 @@
         <v>222</v>
       </c>
       <c r="E60">
-        <f>MATCH(A60,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A60,'231126'!$A$2:$A$39,0)</f>
         <v>17</v>
       </c>
     </row>
@@ -2940,7 +3700,7 @@
         <v>223</v>
       </c>
       <c r="E61">
-        <f>MATCH(A61,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A61,'231126'!$A$2:$A$39,0)</f>
         <v>21</v>
       </c>
     </row>
@@ -2956,7 +3716,7 @@
         <v>224</v>
       </c>
       <c r="E62">
-        <f>MATCH(A62,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A62,'231126'!$A$2:$A$39,0)</f>
         <v>9</v>
       </c>
     </row>
@@ -2972,7 +3732,7 @@
         <v>225</v>
       </c>
       <c r="E63">
-        <f>MATCH(A63,Sheet!$A$2:$A$39,0)</f>
+        <f>MATCH(A63,'231126'!$A$2:$A$39,0)</f>
         <v>5</v>
       </c>
     </row>

</xml_diff>